<commit_message>
Update relevant article selection
</commit_message>
<xml_diff>
--- a/3-data/output/mpox-linked-pages.xlsx
+++ b/3-data/output/mpox-linked-pages.xlsx
@@ -3104,154 +3104,154 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>Wikipedia:WikiProject Current events/Monkeypox outbreak task force</t>
+          <t>Wikipedia:Protection policy</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>Template:2022–2023 mpox outbreak</t>
+          <t>Wikipedia:WikiProject Current events/Monkeypox outbreak task force</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>Template:Country data Congo</t>
+          <t>Template:2022–2023 mpox outbreak</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>Template:Country data Democratic Republic of the Congo</t>
+          <t>Template:Country data Congo</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>Template:Country data Republic of the Congo</t>
+          <t>Template:Country data Democratic Republic of the Congo</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>Template:Viral cutaneous conditions</t>
+          <t>Template:Country data Republic of the Congo</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>Template:Zoonotic viral diseases</t>
+          <t>Template:Viral cutaneous conditions</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>Template talk:2022–2023 mpox outbreak</t>
+          <t>Template:Zoonotic viral diseases</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>Template talk:Viral cutaneous conditions</t>
+          <t>Template talk:2022–2023 mpox outbreak</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>Template talk:Zoonotic viral diseases</t>
+          <t>Template talk:Viral cutaneous conditions</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>Help:Authority control</t>
+          <t>Template talk:Zoonotic viral diseases</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>Help:IPA/English</t>
+          <t>Help:Authority control</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>Help:Pronunciation respelling key</t>
+          <t>Help:IPA/English</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>Category:2022–2023 mpox outbreak</t>
+          <t>Help:Pronunciation respelling key</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>Category:Articles with LNB identifiers</t>
+          <t>Category:2022–2023 mpox outbreak</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>Category:Use dmy dates from December 2022</t>
+          <t>Category:Articles with LNB identifiers</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>Category:Wikipedia articles in need of updating from May 2023</t>
+          <t>Category:Use dmy dates from December 2022</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>Portal:Medicine</t>
+          <t>Category:Wikipedia articles in need of updating from May 2023</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>Portal:Viruses</t>
+          <t>Portal:Medicine</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>Mpox</t>
+          <t>Portal:Viruses</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>Wikipedia:Categorizing redirects</t>
+          <t>Mpox</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>Wikipedia:Protection policy</t>
+          <t>Wikipedia:Categorizing redirects</t>
         </is>
       </c>
     </row>

</xml_diff>